<commit_message>
feat: Update series codes
</commit_message>
<xml_diff>
--- a/input_series.xlsx
+++ b/input_series.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\BCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6259A3EF-2F95-4993-9690-E8C5D99A9691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A4B99D-3589-4600-ACE4-ABA5E660376C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="304">
   <si>
     <t>Codigo</t>
   </si>
@@ -926,6 +939,12 @@
   </si>
   <si>
     <t>21403</t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>BK</t>
   </si>
 </sst>
 </file>
@@ -961,10 +980,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1305,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C253"/>
+  <dimension ref="A1:C258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1894,8 +1916,8 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>87</v>
+      <c r="A54" s="1">
+        <v>20881</v>
       </c>
       <c r="B54" t="s">
         <v>39</v>
@@ -1906,7 +1928,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
         <v>41</v>
@@ -1917,7 +1939,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
         <v>43</v>
@@ -1928,7 +1950,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B57" t="s">
         <v>45</v>
@@ -1939,7 +1961,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B58" t="s">
         <v>47</v>
@@ -1950,7 +1972,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
         <v>49</v>
@@ -1961,7 +1983,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B60" t="s">
         <v>51</v>
@@ -1972,7 +1994,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
         <v>53</v>
@@ -1983,7 +2005,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B62" t="s">
         <v>55</v>
@@ -1994,7 +2016,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B63" t="s">
         <v>57</v>
@@ -2005,7 +2027,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B64" t="s">
         <v>59</v>
@@ -2016,7 +2038,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
         <v>61</v>
@@ -2027,7 +2049,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B66" t="s">
         <v>63</v>
@@ -2037,22 +2059,22 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
+      <c r="A67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
         <v>20542</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>6</v>
-      </c>
-      <c r="C67" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>101</v>
-      </c>
-      <c r="B68" t="s">
-        <v>8</v>
       </c>
       <c r="C68" t="s">
         <v>100</v>
@@ -2060,10 +2082,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C69" t="s">
         <v>100</v>
@@ -2071,10 +2093,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B70" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C70" t="s">
         <v>100</v>
@@ -2082,10 +2104,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B71" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C71" t="s">
         <v>100</v>
@@ -2093,10 +2115,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C72" t="s">
         <v>100</v>
@@ -2104,10 +2126,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B73" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C73" t="s">
         <v>100</v>
@@ -2115,10 +2137,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B74" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C74" t="s">
         <v>100</v>
@@ -2126,10 +2148,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B75" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C75" t="s">
         <v>100</v>
@@ -2137,10 +2159,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C76" t="s">
         <v>100</v>
@@ -2148,10 +2170,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B77" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C77" t="s">
         <v>100</v>
@@ -2159,10 +2181,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B78" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C78" t="s">
         <v>100</v>
@@ -2170,10 +2192,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B79" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C79" t="s">
         <v>100</v>
@@ -2181,10 +2203,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B80" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C80" t="s">
         <v>100</v>
@@ -2192,10 +2214,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C81" t="s">
         <v>100</v>
@@ -2203,10 +2225,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B82" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C82" t="s">
         <v>100</v>
@@ -2214,10 +2236,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C83" t="s">
         <v>100</v>
@@ -2225,10 +2247,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B84" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C84" t="s">
         <v>100</v>
@@ -2236,10 +2258,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B85" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C85" t="s">
         <v>100</v>
@@ -2250,664 +2272,664 @@
         <v>104</v>
       </c>
       <c r="B86" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C86" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>104</v>
+      </c>
       <c r="B87" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C87" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>118</v>
-      </c>
       <c r="B88" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C88" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="A89" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B89" t="s">
+        <v>63</v>
+      </c>
+      <c r="C89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>6</v>
-      </c>
-      <c r="C89" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>121</v>
-      </c>
-      <c r="B90" t="s">
-        <v>8</v>
       </c>
       <c r="C90" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>122</v>
+      <c r="A91" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="B91" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C91" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>123</v>
+      <c r="A92" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="B92" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C92" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>124</v>
+      <c r="A93" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="B93" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C93" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>125</v>
+      <c r="A94" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C94" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>126</v>
+      <c r="A95" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="B95" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C95" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>104</v>
+      <c r="A96" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="B96" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C96" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>127</v>
+      <c r="A97" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B97" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C97" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>128</v>
+      <c r="A98" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="B98" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C98" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>129</v>
+      <c r="A99" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="B99" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C99" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>130</v>
+      <c r="A100" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="B100" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C100" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>131</v>
+      <c r="A101" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="B101" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C101" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>132</v>
+      <c r="A102" s="2">
+        <v>20576</v>
       </c>
       <c r="B102" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C102" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>133</v>
+      <c r="A103" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="B103" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C103" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>134</v>
+      <c r="A104" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="B104" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C104" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>135</v>
+      <c r="A105" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="B105" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C105" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>136</v>
+      <c r="A106" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="B106" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C106" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>137</v>
+      <c r="A107" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B107" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C107" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>104</v>
+      <c r="A108" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="B108" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C108" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>138</v>
+      <c r="A109" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="B109" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C109" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>139</v>
+      <c r="A110" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B110" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C110" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>140</v>
+      <c r="A111" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="B111" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C111" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>141</v>
+      <c r="A112" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="B112" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C112" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>142</v>
+      <c r="A113" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="B113" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C113" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>143</v>
+      <c r="A114" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="B114" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C114" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>144</v>
+      <c r="A115" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="B115" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C115" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>145</v>
+      <c r="A116" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="B116" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C116" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>146</v>
+      <c r="A117" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="B117" t="s">
-        <v>147</v>
+        <v>75</v>
       </c>
       <c r="C117" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>148</v>
+      <c r="A118" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="B118" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C118" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>150</v>
+      <c r="A119" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="B119" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C119" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="A120" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B120" t="s">
+        <v>151</v>
+      </c>
+      <c r="C120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B121" t="s">
+        <v>210</v>
+      </c>
+      <c r="C121" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B122" t="s">
         <v>4</v>
-      </c>
-      <c r="C120" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>154</v>
-      </c>
-      <c r="B121" t="s">
-        <v>6</v>
-      </c>
-      <c r="C121" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>155</v>
-      </c>
-      <c r="B122" t="s">
-        <v>8</v>
       </c>
       <c r="C122" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+      <c r="A123" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B123" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B124" t="s">
+        <v>8</v>
+      </c>
+      <c r="C124" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B123" t="s">
-        <v>4</v>
-      </c>
-      <c r="C123" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>158</v>
-      </c>
-      <c r="B124" t="s">
-        <v>6</v>
-      </c>
-      <c r="C124" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>159</v>
       </c>
       <c r="B125" t="s">
         <v>4</v>
       </c>
       <c r="C125" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>161</v>
+      <c r="A126" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
       </c>
       <c r="C126" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>162</v>
+      <c r="A127" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="B127" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C127" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>163</v>
+      <c r="A128" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="B128" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C128" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>164</v>
+      <c r="A129" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="B129" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C129" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
-        <v>165</v>
+      <c r="A130" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="B130" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C130" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>166</v>
+      <c r="A131" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="B131" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C131" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>167</v>
+      <c r="A132" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="B132" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C132" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>168</v>
+      <c r="A133" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="B133" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C133" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>169</v>
+      <c r="A134" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="B134" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C134" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>170</v>
+      <c r="A135" s="2">
+        <v>20744</v>
       </c>
       <c r="B135" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C135" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>171</v>
+      <c r="A136" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="B136" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C136" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>172</v>
+      <c r="A137" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="B137" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C137" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>173</v>
+      <c r="A138" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="B138" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C138" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>174</v>
+      <c r="A139" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="B139" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C139" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>175</v>
+      <c r="A140" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="B140" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C140" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>176</v>
+      <c r="A141" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="B141" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C141" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>177</v>
+      <c r="A142" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="B142" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C142" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>178</v>
+      <c r="A143" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="B143" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C143" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>180</v>
+      <c r="A144" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="B144" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C144" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>181</v>
+      <c r="A145" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="B145" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="C145" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B146" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C146" t="s">
         <v>179</v>
@@ -2915,10 +2937,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B147" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C147" t="s">
         <v>179</v>
@@ -2926,10 +2948,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B148" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C148" t="s">
         <v>179</v>
@@ -2937,10 +2959,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="B149" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C149" t="s">
         <v>179</v>
@@ -2948,10 +2970,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B150" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C150" t="s">
         <v>179</v>
@@ -2959,10 +2981,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B151" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C151" t="s">
         <v>179</v>
@@ -2970,10 +2992,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>187</v>
+        <v>104</v>
       </c>
       <c r="B152" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C152" t="s">
         <v>179</v>
@@ -2981,10 +3003,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B153" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C153" t="s">
         <v>179</v>
@@ -2992,10 +3014,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B154" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C154" t="s">
         <v>179</v>
@@ -3003,10 +3025,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B155" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C155" t="s">
         <v>179</v>
@@ -3014,10 +3036,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B156" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C156" t="s">
         <v>179</v>
@@ -3025,10 +3047,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B157" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C157" t="s">
         <v>179</v>
@@ -3036,10 +3058,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B158" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C158" t="s">
         <v>179</v>
@@ -3047,10 +3069,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B159" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C159" t="s">
         <v>179</v>
@@ -3058,10 +3080,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B160" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C160" t="s">
         <v>179</v>
@@ -3069,10 +3091,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B161" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C161" t="s">
         <v>179</v>
@@ -3080,10 +3102,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B162" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C162" t="s">
         <v>179</v>
@@ -3091,10 +3113,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B163" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C163" t="s">
         <v>179</v>
@@ -3102,21 +3124,21 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B164" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C164" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
-        <v>200</v>
+      <c r="A165">
+        <v>21037</v>
       </c>
       <c r="B165" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C165" t="s">
         <v>179</v>
@@ -3124,10 +3146,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B166" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C166" t="s">
         <v>179</v>
@@ -3135,10 +3157,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B167" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C167" t="s">
         <v>179</v>
@@ -3146,10 +3168,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B168" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C168" t="s">
         <v>179</v>
@@ -3157,10 +3179,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B169" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C169" t="s">
         <v>179</v>
@@ -3168,10 +3190,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B170" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C170" t="s">
         <v>179</v>
@@ -3179,10 +3201,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B171" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C171" t="s">
         <v>179</v>
@@ -3190,10 +3212,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>104</v>
+        <v>203</v>
       </c>
       <c r="B172" t="s">
-        <v>147</v>
+        <v>71</v>
       </c>
       <c r="C172" t="s">
         <v>179</v>
@@ -3201,10 +3223,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B173" t="s">
-        <v>149</v>
+        <v>73</v>
       </c>
       <c r="C173" t="s">
         <v>179</v>
@@ -3212,10 +3234,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B174" t="s">
-        <v>151</v>
+        <v>75</v>
       </c>
       <c r="C174" t="s">
         <v>179</v>
@@ -3223,10 +3245,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B175" t="s">
-        <v>210</v>
+        <v>147</v>
       </c>
       <c r="C175" t="s">
         <v>179</v>
@@ -3234,10 +3256,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>211</v>
+        <v>104</v>
       </c>
       <c r="B176" t="s">
-        <v>212</v>
+        <v>149</v>
       </c>
       <c r="C176" t="s">
         <v>179</v>
@@ -3245,10 +3267,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B177" t="s">
-        <v>214</v>
+        <v>151</v>
       </c>
       <c r="C177" t="s">
         <v>179</v>
@@ -3256,10 +3278,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B178" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="C178" t="s">
         <v>179</v>
@@ -3267,10 +3289,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B179" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C179" t="s">
         <v>179</v>
@@ -3278,10 +3300,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B180" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C180" t="s">
         <v>179</v>
@@ -3289,10 +3311,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B181" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C181" t="s">
         <v>179</v>
@@ -3300,10 +3322,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B182" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C182" t="s">
         <v>179</v>
@@ -3311,10 +3333,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B183" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C183" t="s">
         <v>179</v>
@@ -3322,10 +3344,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B184" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C184" t="s">
         <v>179</v>
@@ -3333,10 +3355,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B185" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C185" t="s">
         <v>179</v>
@@ -3344,10 +3366,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B186" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C186" t="s">
         <v>179</v>
@@ -3355,10 +3377,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B187" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C187" t="s">
         <v>179</v>
@@ -3366,10 +3388,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B188" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C188" t="s">
         <v>179</v>
@@ -3377,10 +3399,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B189" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C189" t="s">
         <v>179</v>
@@ -3388,10 +3410,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B190" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C190" t="s">
         <v>179</v>
@@ -3399,21 +3421,21 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B191" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C191" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A192" t="s">
-        <v>243</v>
+      <c r="A192">
+        <v>21116</v>
       </c>
       <c r="B192" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C192" t="s">
         <v>179</v>
@@ -3421,10 +3443,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B193" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C193" t="s">
         <v>179</v>
@@ -3432,10 +3454,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B194" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C194" t="s">
         <v>179</v>
@@ -3443,10 +3465,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B195" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C195" t="s">
         <v>179</v>
@@ -3454,10 +3476,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B196" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C196" t="s">
         <v>179</v>
@@ -3465,10 +3487,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B197" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C197" t="s">
         <v>179</v>
@@ -3476,10 +3498,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>104</v>
+        <v>245</v>
       </c>
       <c r="B198" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C198" t="s">
         <v>179</v>
@@ -3487,10 +3509,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B199" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C199" t="s">
         <v>179</v>
@@ -3498,10 +3520,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B200" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C200" t="s">
         <v>179</v>
@@ -3509,10 +3531,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B201" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C201" t="s">
         <v>179</v>
@@ -3520,10 +3542,10 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B202" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C202" t="s">
         <v>179</v>
@@ -3531,65 +3553,65 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>213</v>
+        <v>104</v>
       </c>
       <c r="B203" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
       <c r="C203" t="s">
-        <v>264</v>
+        <v>179</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B204" t="s">
-        <v>6</v>
+        <v>261</v>
       </c>
       <c r="C204" t="s">
-        <v>264</v>
+        <v>179</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B205" t="s">
-        <v>8</v>
+        <v>263</v>
       </c>
       <c r="C205" t="s">
-        <v>264</v>
+        <v>179</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>104</v>
+        <v>260</v>
       </c>
       <c r="B206" t="s">
-        <v>10</v>
+        <v>302</v>
       </c>
       <c r="C206" t="s">
-        <v>264</v>
+        <v>179</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B207" t="s">
-        <v>16</v>
+        <v>303</v>
       </c>
       <c r="C207" t="s">
-        <v>264</v>
+        <v>179</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>268</v>
+        <v>213</v>
       </c>
       <c r="B208" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C208" t="s">
         <v>264</v>
@@ -3597,10 +3619,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B209" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C209" t="s">
         <v>264</v>
@@ -3608,65 +3630,65 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B210" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C210" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>272</v>
+        <v>104</v>
       </c>
       <c r="B211" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C211" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>104</v>
+        <v>267</v>
       </c>
       <c r="B212" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C212" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B213" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C213" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>104</v>
+        <v>269</v>
       </c>
       <c r="B214" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C214" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B215" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C215" t="s">
         <v>271</v>
@@ -3674,10 +3696,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B216" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C216" t="s">
         <v>271</v>
@@ -3688,7 +3710,7 @@
         <v>104</v>
       </c>
       <c r="B217" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C217" t="s">
         <v>271</v>
@@ -3696,10 +3718,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>104</v>
+        <v>273</v>
       </c>
       <c r="B218" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C218" t="s">
         <v>271</v>
@@ -3710,7 +3732,7 @@
         <v>104</v>
       </c>
       <c r="B219" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C219" t="s">
         <v>271</v>
@@ -3718,10 +3740,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>104</v>
+        <v>274</v>
       </c>
       <c r="B220" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C220" t="s">
         <v>271</v>
@@ -3729,10 +3751,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>104</v>
+        <v>275</v>
       </c>
       <c r="B221" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C221" t="s">
         <v>271</v>
@@ -3740,10 +3762,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>276</v>
+        <v>104</v>
       </c>
       <c r="B222" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C222" t="s">
         <v>271</v>
@@ -3751,24 +3773,24 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>277</v>
+        <v>104</v>
       </c>
       <c r="B223" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C223" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>279</v>
+        <v>104</v>
       </c>
       <c r="B224" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C224" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
@@ -3776,40 +3798,40 @@
         <v>104</v>
       </c>
       <c r="B225" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C225" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>280</v>
+        <v>104</v>
       </c>
       <c r="B226" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C226" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B227" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C227" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>104</v>
+        <v>277</v>
       </c>
       <c r="B228" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C228" t="s">
         <v>278</v>
@@ -3817,10 +3839,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B229" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C229" t="s">
         <v>278</v>
@@ -3828,10 +3850,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>283</v>
+        <v>104</v>
       </c>
       <c r="B230" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C230" t="s">
         <v>278</v>
@@ -3839,10 +3861,10 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>104</v>
+        <v>280</v>
       </c>
       <c r="B231" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C231" t="s">
         <v>278</v>
@@ -3850,10 +3872,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B232" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C232" t="s">
         <v>278</v>
@@ -3861,10 +3883,10 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>285</v>
+        <v>104</v>
       </c>
       <c r="B233" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C233" t="s">
         <v>278</v>
@@ -3872,10 +3894,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>104</v>
+        <v>282</v>
       </c>
       <c r="B234" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C234" t="s">
         <v>278</v>
@@ -3883,10 +3905,10 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B235" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C235" t="s">
         <v>278</v>
@@ -3894,10 +3916,10 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>287</v>
+        <v>104</v>
       </c>
       <c r="B236" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C236" t="s">
         <v>278</v>
@@ -3905,10 +3927,10 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B237" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C237" t="s">
         <v>278</v>
@@ -3916,10 +3938,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B238" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C238" t="s">
         <v>278</v>
@@ -3927,10 +3949,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>290</v>
+        <v>104</v>
       </c>
       <c r="B239" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C239" t="s">
         <v>278</v>
@@ -3938,10 +3960,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B240" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C240" t="s">
         <v>278</v>
@@ -3949,10 +3971,10 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B241" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C241" t="s">
         <v>278</v>
@@ -3960,10 +3982,10 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B242" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C242" t="s">
         <v>278</v>
@@ -3971,10 +3993,10 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B243" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C243" t="s">
         <v>278</v>
@@ -3982,10 +4004,10 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B244" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C244" t="s">
         <v>278</v>
@@ -3993,10 +4015,10 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>104</v>
+        <v>291</v>
       </c>
       <c r="B245" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C245" t="s">
         <v>278</v>
@@ -4004,10 +4026,10 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B246" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C246" t="s">
         <v>278</v>
@@ -4015,10 +4037,10 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B247" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C247" t="s">
         <v>278</v>
@@ -4026,10 +4048,10 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>104</v>
+        <v>294</v>
       </c>
       <c r="B248" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C248" t="s">
         <v>278</v>
@@ -4037,10 +4059,10 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B249" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C249" t="s">
         <v>278</v>
@@ -4048,10 +4070,10 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>299</v>
+        <v>104</v>
       </c>
       <c r="B250" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C250" t="s">
         <v>278</v>
@@ -4059,10 +4081,10 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>104</v>
+        <v>296</v>
       </c>
       <c r="B251" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C251" t="s">
         <v>278</v>
@@ -4070,10 +4092,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B252" t="s">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="C252" t="s">
         <v>278</v>
@@ -4081,19 +4103,74 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
+        <v>104</v>
+      </c>
+      <c r="B253" t="s">
+        <v>69</v>
+      </c>
+      <c r="C253" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>298</v>
+      </c>
+      <c r="B254" t="s">
+        <v>71</v>
+      </c>
+      <c r="C254" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>299</v>
+      </c>
+      <c r="B255" t="s">
+        <v>73</v>
+      </c>
+      <c r="C255" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>104</v>
+      </c>
+      <c r="B256" t="s">
+        <v>75</v>
+      </c>
+      <c r="C256" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>300</v>
+      </c>
+      <c r="B257" t="s">
+        <v>147</v>
+      </c>
+      <c r="C257" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
         <v>301</v>
       </c>
-      <c r="B253" t="s">
+      <c r="B258" t="s">
         <v>149</v>
       </c>
-      <c r="C253" t="s">
+      <c r="C258" t="s">
         <v>278</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C66 A68:C253 B67:C67" numberStoredAsText="1"/>
+    <ignoredError sqref="A208:C258 B68:C68 A1:C53 A55:A67 C55:C67 A69:C101 A103:A121 C103:C121 A122:C134 A136:A145 C136:C145 A146:C164 A193:A206 C193:C206 C166:C191 A166:A191 A207 C207" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Implement post-processing to rename DataFrame columns to series codes.
</commit_message>
<xml_diff>
--- a/input_series.xlsx
+++ b/input_series.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\BCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A4B99D-3589-4600-ACE4-ABA5E660376C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A508765-2F3C-4F56-877C-C215A45C33EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -985,8 +985,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1329,14 +1329,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.796875" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1347,7 +1350,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -1358,6 +1361,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -1366,7 +1370,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
@@ -1377,7 +1381,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
@@ -1388,7 +1392,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
@@ -1399,7 +1403,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
@@ -1410,7 +1414,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
@@ -1421,7 +1425,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
@@ -1432,7 +1436,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
@@ -1443,7 +1447,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
@@ -1454,7 +1458,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B12" t="s">
@@ -1465,7 +1469,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
@@ -1476,7 +1480,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
@@ -1487,7 +1491,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
@@ -1498,7 +1502,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B16" t="s">
@@ -1509,7 +1513,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B17" t="s">
@@ -1520,7 +1524,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B18" t="s">
@@ -1531,7 +1535,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B19" t="s">
@@ -1542,7 +1546,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B20" t="s">
@@ -1553,7 +1557,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B21" t="s">
@@ -1564,7 +1568,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B22" t="s">
@@ -1575,7 +1579,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B23" t="s">
@@ -1586,7 +1590,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B24" t="s">
@@ -1597,7 +1601,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B25" t="s">
@@ -1608,7 +1612,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B26" t="s">
@@ -1619,7 +1623,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B27" t="s">
@@ -1630,7 +1634,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B28" t="s">
@@ -1641,7 +1645,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B29" t="s">
@@ -1652,7 +1656,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B30" t="s">
@@ -1663,7 +1667,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B31" t="s">
@@ -1674,7 +1678,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B32" t="s">
@@ -1685,7 +1689,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B33" t="s">
@@ -1696,7 +1700,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B34" t="s">
@@ -1707,7 +1711,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B35" t="s">
@@ -1718,7 +1722,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B36" t="s">
@@ -1729,7 +1733,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B37" t="s">
@@ -1740,7 +1744,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B38" t="s">
@@ -1751,7 +1755,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B39" t="s">
@@ -1762,7 +1766,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B40" t="s">
@@ -1773,7 +1777,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B41" t="s">
@@ -1784,7 +1788,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B42" t="s">
@@ -1795,7 +1799,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B43" t="s">
@@ -1806,7 +1810,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B44" t="s">
@@ -1817,7 +1821,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B45" t="s">
@@ -1828,7 +1832,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B46" t="s">
@@ -1839,7 +1843,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B47" t="s">
@@ -1850,7 +1854,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B48" t="s">
@@ -1861,7 +1865,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B49" t="s">
@@ -1872,7 +1876,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B50" t="s">
@@ -1883,7 +1887,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B51" t="s">
@@ -1894,7 +1898,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B52" t="s">
@@ -1905,7 +1909,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B53" t="s">
@@ -1916,7 +1920,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
+      <c r="A54" s="2">
         <v>20881</v>
       </c>
       <c r="B54" t="s">
@@ -1927,7 +1931,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B55" t="s">
@@ -1938,7 +1942,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="A56" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B56" t="s">
@@ -1949,7 +1953,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B57" t="s">
@@ -1960,7 +1964,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B58" t="s">
@@ -1971,7 +1975,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B59" t="s">
@@ -1982,7 +1986,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="A60" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B60" t="s">
@@ -1993,7 +1997,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B61" t="s">
@@ -2004,7 +2008,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="A62" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B62" t="s">
@@ -2015,7 +2019,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="A63" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B63" t="s">
@@ -2026,7 +2030,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="A64" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B64" t="s">
@@ -2037,7 +2041,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="A65" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B65" t="s">
@@ -2048,7 +2052,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="A66" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B66" t="s">
@@ -2059,7 +2063,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="A67" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B67" t="s">
@@ -2070,7 +2074,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
+      <c r="A68" s="2">
         <v>20542</v>
       </c>
       <c r="B68" t="s">
@@ -2081,7 +2085,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="A69" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B69" t="s">
@@ -2092,7 +2096,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="A70" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B70" t="s">
@@ -2103,7 +2107,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="A71" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B71" t="s">
@@ -2114,7 +2118,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+      <c r="A72" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B72" t="s">
@@ -2125,7 +2129,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="A73" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B73" t="s">
@@ -2136,7 +2140,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+      <c r="A74" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B74" t="s">
@@ -2147,7 +2151,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+      <c r="A75" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B75" t="s">
@@ -2158,7 +2162,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+      <c r="A76" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B76" t="s">
@@ -2169,7 +2173,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="A77" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B77" t="s">
@@ -2180,7 +2184,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="A78" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B78" t="s">
@@ -2191,7 +2195,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="A79" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B79" t="s">
@@ -2202,7 +2206,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+      <c r="A80" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B80" t="s">
@@ -2213,7 +2217,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="A81" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B81" t="s">
@@ -2224,7 +2228,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="A82" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B82" t="s">
@@ -2235,7 +2239,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="A83" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B83" t="s">
@@ -2246,7 +2250,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="A84" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B84" t="s">
@@ -2257,7 +2261,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="A85" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B85" t="s">
@@ -2268,7 +2272,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="A86" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B86" t="s">
@@ -2279,7 +2283,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="A87" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B87" t="s">
@@ -2290,6 +2294,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="2"/>
       <c r="B88" t="s">
         <v>61</v>
       </c>
@@ -2925,7 +2930,7 @@
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+      <c r="A146" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B146" t="s">
@@ -2936,7 +2941,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+      <c r="A147" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B147" t="s">
@@ -2947,7 +2952,7 @@
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
+      <c r="A148" s="2" t="s">
         <v>181</v>
       </c>
       <c r="B148" t="s">
@@ -2958,7 +2963,7 @@
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
+      <c r="A149" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B149" t="s">
@@ -2969,7 +2974,7 @@
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
+      <c r="A150" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B150" t="s">
@@ -2980,7 +2985,7 @@
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
+      <c r="A151" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B151" t="s">
@@ -2991,7 +2996,7 @@
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
+      <c r="A152" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B152" t="s">
@@ -3002,7 +3007,7 @@
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
+      <c r="A153" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B153" t="s">
@@ -3013,7 +3018,7 @@
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
+      <c r="A154" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B154" t="s">
@@ -3024,7 +3029,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
+      <c r="A155" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B155" t="s">
@@ -3035,7 +3040,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
+      <c r="A156" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B156" t="s">
@@ -3046,7 +3051,7 @@
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
+      <c r="A157" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B157" t="s">
@@ -3057,7 +3062,7 @@
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
+      <c r="A158" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B158" t="s">
@@ -3068,7 +3073,7 @@
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
+      <c r="A159" s="2" t="s">
         <v>191</v>
       </c>
       <c r="B159" t="s">
@@ -3079,7 +3084,7 @@
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
+      <c r="A160" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B160" t="s">
@@ -3090,7 +3095,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+      <c r="A161" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B161" t="s">
@@ -3101,7 +3106,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
+      <c r="A162" s="2" t="s">
         <v>194</v>
       </c>
       <c r="B162" t="s">
@@ -3112,7 +3117,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
+      <c r="A163" s="2" t="s">
         <v>195</v>
       </c>
       <c r="B163" t="s">
@@ -3123,7 +3128,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
+      <c r="A164" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B164" t="s">
@@ -3134,7 +3139,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165">
+      <c r="A165" s="2">
         <v>21037</v>
       </c>
       <c r="B165" t="s">
@@ -3145,7 +3150,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
+      <c r="A166" s="2" t="s">
         <v>197</v>
       </c>
       <c r="B166" t="s">
@@ -3156,7 +3161,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
+      <c r="A167" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B167" t="s">
@@ -3167,7 +3172,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
+      <c r="A168" s="2" t="s">
         <v>199</v>
       </c>
       <c r="B168" t="s">
@@ -3178,7 +3183,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
+      <c r="A169" s="2" t="s">
         <v>200</v>
       </c>
       <c r="B169" t="s">
@@ -3189,7 +3194,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
+      <c r="A170" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B170" t="s">
@@ -3200,7 +3205,7 @@
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
+      <c r="A171" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B171" t="s">
@@ -3211,7 +3216,7 @@
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
+      <c r="A172" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B172" t="s">
@@ -3222,7 +3227,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
+      <c r="A173" s="2" t="s">
         <v>204</v>
       </c>
       <c r="B173" t="s">
@@ -3233,7 +3238,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
+      <c r="A174" s="2" t="s">
         <v>205</v>
       </c>
       <c r="B174" t="s">
@@ -3244,7 +3249,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
+      <c r="A175" s="2" t="s">
         <v>206</v>
       </c>
       <c r="B175" t="s">
@@ -3255,7 +3260,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
+      <c r="A176" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B176" t="s">
@@ -3266,7 +3271,7 @@
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A177" t="s">
+      <c r="A177" s="2" t="s">
         <v>207</v>
       </c>
       <c r="B177" t="s">
@@ -3277,7 +3282,7 @@
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A178" t="s">
+      <c r="A178" s="2" t="s">
         <v>208</v>
       </c>
       <c r="B178" t="s">
@@ -3288,7 +3293,7 @@
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" t="s">
+      <c r="A179" s="2" t="s">
         <v>209</v>
       </c>
       <c r="B179" t="s">
@@ -3299,7 +3304,7 @@
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
+      <c r="A180" s="2" t="s">
         <v>211</v>
       </c>
       <c r="B180" t="s">
@@ -3310,7 +3315,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A181" t="s">
+      <c r="A181" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B181" t="s">
@@ -3321,7 +3326,7 @@
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A182" t="s">
+      <c r="A182" s="2" t="s">
         <v>215</v>
       </c>
       <c r="B182" t="s">
@@ -3332,7 +3337,7 @@
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183" t="s">
+      <c r="A183" s="2" t="s">
         <v>217</v>
       </c>
       <c r="B183" t="s">
@@ -3343,7 +3348,7 @@
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
+      <c r="A184" s="2" t="s">
         <v>219</v>
       </c>
       <c r="B184" t="s">
@@ -3354,7 +3359,7 @@
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A185" t="s">
+      <c r="A185" s="2" t="s">
         <v>221</v>
       </c>
       <c r="B185" t="s">
@@ -3365,7 +3370,7 @@
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
+      <c r="A186" s="2" t="s">
         <v>223</v>
       </c>
       <c r="B186" t="s">
@@ -3376,7 +3381,7 @@
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
+      <c r="A187" s="2" t="s">
         <v>225</v>
       </c>
       <c r="B187" t="s">
@@ -3387,7 +3392,7 @@
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
+      <c r="A188" s="2" t="s">
         <v>227</v>
       </c>
       <c r="B188" t="s">
@@ -3398,7 +3403,7 @@
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A189" t="s">
+      <c r="A189" s="2" t="s">
         <v>229</v>
       </c>
       <c r="B189" t="s">
@@ -3409,7 +3414,7 @@
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A190" t="s">
+      <c r="A190" s="2" t="s">
         <v>231</v>
       </c>
       <c r="B190" t="s">
@@ -3420,7 +3425,7 @@
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
+      <c r="A191" s="2" t="s">
         <v>233</v>
       </c>
       <c r="B191" t="s">
@@ -3431,7 +3436,7 @@
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A192">
+      <c r="A192" s="2">
         <v>21116</v>
       </c>
       <c r="B192" t="s">
@@ -3442,7 +3447,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" t="s">
+      <c r="A193" s="2" t="s">
         <v>235</v>
       </c>
       <c r="B193" t="s">
@@ -3453,7 +3458,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" t="s">
+      <c r="A194" s="2" t="s">
         <v>237</v>
       </c>
       <c r="B194" t="s">
@@ -3464,7 +3469,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" t="s">
+      <c r="A195" s="2" t="s">
         <v>239</v>
       </c>
       <c r="B195" t="s">
@@ -3475,7 +3480,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
+      <c r="A196" s="2" t="s">
         <v>241</v>
       </c>
       <c r="B196" t="s">
@@ -3486,7 +3491,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" t="s">
+      <c r="A197" s="2" t="s">
         <v>243</v>
       </c>
       <c r="B197" t="s">
@@ -3497,7 +3502,7 @@
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A198" t="s">
+      <c r="A198" s="2" t="s">
         <v>245</v>
       </c>
       <c r="B198" t="s">
@@ -3508,7 +3513,7 @@
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A199" t="s">
+      <c r="A199" s="2" t="s">
         <v>247</v>
       </c>
       <c r="B199" t="s">
@@ -3519,7 +3524,7 @@
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
+      <c r="A200" s="2" t="s">
         <v>249</v>
       </c>
       <c r="B200" t="s">
@@ -3530,7 +3535,7 @@
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
+      <c r="A201" s="2" t="s">
         <v>251</v>
       </c>
       <c r="B201" t="s">
@@ -3541,7 +3546,7 @@
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
+      <c r="A202" s="2" t="s">
         <v>253</v>
       </c>
       <c r="B202" t="s">
@@ -3552,7 +3557,7 @@
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A203" t="s">
+      <c r="A203" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B203" t="s">
@@ -3563,7 +3568,7 @@
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A204" t="s">
+      <c r="A204" s="2" t="s">
         <v>256</v>
       </c>
       <c r="B204" t="s">
@@ -3574,7 +3579,7 @@
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A205" t="s">
+      <c r="A205" s="2" t="s">
         <v>258</v>
       </c>
       <c r="B205" t="s">
@@ -3585,7 +3590,7 @@
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
+      <c r="A206" s="2" t="s">
         <v>260</v>
       </c>
       <c r="B206" t="s">
@@ -3596,7 +3601,7 @@
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A207" t="s">
+      <c r="A207" s="2" t="s">
         <v>262</v>
       </c>
       <c r="B207" t="s">
@@ -3607,7 +3612,7 @@
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A208" t="s">
+      <c r="A208" s="2" t="s">
         <v>213</v>
       </c>
       <c r="B208" t="s">
@@ -3618,7 +3623,7 @@
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A209" t="s">
+      <c r="A209" s="2" t="s">
         <v>265</v>
       </c>
       <c r="B209" t="s">
@@ -3629,7 +3634,7 @@
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A210" t="s">
+      <c r="A210" s="2" t="s">
         <v>266</v>
       </c>
       <c r="B210" t="s">
@@ -3640,7 +3645,7 @@
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A211" t="s">
+      <c r="A211" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B211" t="s">
@@ -3651,7 +3656,7 @@
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A212" t="s">
+      <c r="A212" s="2" t="s">
         <v>267</v>
       </c>
       <c r="B212" t="s">
@@ -3662,7 +3667,7 @@
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A213" t="s">
+      <c r="A213" s="2" t="s">
         <v>268</v>
       </c>
       <c r="B213" t="s">
@@ -3673,7 +3678,7 @@
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A214" t="s">
+      <c r="A214" s="2" t="s">
         <v>269</v>
       </c>
       <c r="B214" t="s">
@@ -3684,7 +3689,7 @@
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A215" t="s">
+      <c r="A215" s="2" t="s">
         <v>270</v>
       </c>
       <c r="B215" t="s">
@@ -3695,7 +3700,7 @@
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A216" t="s">
+      <c r="A216" s="2" t="s">
         <v>272</v>
       </c>
       <c r="B216" t="s">
@@ -3706,7 +3711,7 @@
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A217" t="s">
+      <c r="A217" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B217" t="s">
@@ -3717,7 +3722,7 @@
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A218" t="s">
+      <c r="A218" s="2" t="s">
         <v>273</v>
       </c>
       <c r="B218" t="s">
@@ -3728,7 +3733,7 @@
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A219" t="s">
+      <c r="A219" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B219" t="s">
@@ -3739,7 +3744,7 @@
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A220" t="s">
+      <c r="A220" s="2" t="s">
         <v>274</v>
       </c>
       <c r="B220" t="s">
@@ -3750,7 +3755,7 @@
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A221" t="s">
+      <c r="A221" s="2" t="s">
         <v>275</v>
       </c>
       <c r="B221" t="s">
@@ -3761,7 +3766,7 @@
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A222" t="s">
+      <c r="A222" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B222" t="s">
@@ -3772,7 +3777,7 @@
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A223" t="s">
+      <c r="A223" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B223" t="s">
@@ -3783,7 +3788,7 @@
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A224" t="s">
+      <c r="A224" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B224" t="s">
@@ -3794,7 +3799,7 @@
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A225" t="s">
+      <c r="A225" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B225" t="s">
@@ -3805,7 +3810,7 @@
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A226" t="s">
+      <c r="A226" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B226" t="s">
@@ -3816,7 +3821,7 @@
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A227" t="s">
+      <c r="A227" s="2" t="s">
         <v>276</v>
       </c>
       <c r="B227" t="s">
@@ -3827,7 +3832,7 @@
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A228" t="s">
+      <c r="A228" s="2" t="s">
         <v>277</v>
       </c>
       <c r="B228" t="s">
@@ -3838,7 +3843,7 @@
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A229" t="s">
+      <c r="A229" s="2" t="s">
         <v>279</v>
       </c>
       <c r="B229" t="s">
@@ -3849,7 +3854,7 @@
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A230" t="s">
+      <c r="A230" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B230" t="s">
@@ -3860,7 +3865,7 @@
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A231" t="s">
+      <c r="A231" s="2" t="s">
         <v>280</v>
       </c>
       <c r="B231" t="s">
@@ -3871,7 +3876,7 @@
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A232" t="s">
+      <c r="A232" s="2" t="s">
         <v>281</v>
       </c>
       <c r="B232" t="s">
@@ -3882,7 +3887,7 @@
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A233" t="s">
+      <c r="A233" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B233" t="s">
@@ -3893,7 +3898,7 @@
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A234" t="s">
+      <c r="A234" s="2" t="s">
         <v>282</v>
       </c>
       <c r="B234" t="s">
@@ -3904,7 +3909,7 @@
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A235" t="s">
+      <c r="A235" s="2" t="s">
         <v>283</v>
       </c>
       <c r="B235" t="s">
@@ -3915,7 +3920,7 @@
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A236" t="s">
+      <c r="A236" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B236" t="s">
@@ -3926,7 +3931,7 @@
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A237" t="s">
+      <c r="A237" s="2" t="s">
         <v>284</v>
       </c>
       <c r="B237" t="s">
@@ -3937,7 +3942,7 @@
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A238" t="s">
+      <c r="A238" s="2" t="s">
         <v>285</v>
       </c>
       <c r="B238" t="s">
@@ -3948,7 +3953,7 @@
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A239" t="s">
+      <c r="A239" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B239" t="s">
@@ -3959,7 +3964,7 @@
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A240" t="s">
+      <c r="A240" s="2" t="s">
         <v>286</v>
       </c>
       <c r="B240" t="s">
@@ -3970,7 +3975,7 @@
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A241" t="s">
+      <c r="A241" s="2" t="s">
         <v>287</v>
       </c>
       <c r="B241" t="s">
@@ -3981,7 +3986,7 @@
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A242" t="s">
+      <c r="A242" s="2" t="s">
         <v>288</v>
       </c>
       <c r="B242" t="s">
@@ -3992,7 +3997,7 @@
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A243" t="s">
+      <c r="A243" s="2" t="s">
         <v>289</v>
       </c>
       <c r="B243" t="s">
@@ -4003,7 +4008,7 @@
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A244" t="s">
+      <c r="A244" s="2" t="s">
         <v>290</v>
       </c>
       <c r="B244" t="s">
@@ -4014,7 +4019,7 @@
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A245" t="s">
+      <c r="A245" s="2" t="s">
         <v>291</v>
       </c>
       <c r="B245" t="s">
@@ -4025,7 +4030,7 @@
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A246" t="s">
+      <c r="A246" s="2" t="s">
         <v>292</v>
       </c>
       <c r="B246" t="s">
@@ -4036,7 +4041,7 @@
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A247" t="s">
+      <c r="A247" s="2" t="s">
         <v>293</v>
       </c>
       <c r="B247" t="s">
@@ -4047,7 +4052,7 @@
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A248" t="s">
+      <c r="A248" s="2" t="s">
         <v>294</v>
       </c>
       <c r="B248" t="s">
@@ -4058,7 +4063,7 @@
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A249" t="s">
+      <c r="A249" s="2" t="s">
         <v>295</v>
       </c>
       <c r="B249" t="s">
@@ -4069,7 +4074,7 @@
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A250" t="s">
+      <c r="A250" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B250" t="s">
@@ -4080,7 +4085,7 @@
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A251" t="s">
+      <c r="A251" s="2" t="s">
         <v>296</v>
       </c>
       <c r="B251" t="s">
@@ -4091,7 +4096,7 @@
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A252" t="s">
+      <c r="A252" s="2" t="s">
         <v>297</v>
       </c>
       <c r="B252" t="s">
@@ -4102,7 +4107,7 @@
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A253" t="s">
+      <c r="A253" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B253" t="s">
@@ -4113,7 +4118,7 @@
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A254" t="s">
+      <c r="A254" s="2" t="s">
         <v>298</v>
       </c>
       <c r="B254" t="s">
@@ -4124,7 +4129,7 @@
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A255" t="s">
+      <c r="A255" s="2" t="s">
         <v>299</v>
       </c>
       <c r="B255" t="s">
@@ -4135,7 +4140,7 @@
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A256" t="s">
+      <c r="A256" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B256" t="s">
@@ -4146,7 +4151,7 @@
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A257" t="s">
+      <c r="A257" s="2" t="s">
         <v>300</v>
       </c>
       <c r="B257" t="s">
@@ -4157,7 +4162,7 @@
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A258" t="s">
+      <c r="A258" s="2" t="s">
         <v>301</v>
       </c>
       <c r="B258" t="s">

</xml_diff>